<commit_message>
Added Stages to raw data
</commit_message>
<xml_diff>
--- a/data/Behavior_Teens_Long.xlsx
+++ b/data/Behavior_Teens_Long.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\IHC\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\LT-AoP-22\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8549E2-DD42-4604-A613-FDDF1A5A06B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C971C2F-2FDD-47A0-846C-BD719515AF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11670" yWindow="2520" windowWidth="13305" windowHeight="11985" xr2:uid="{5020D2FC-34FC-4E93-AA99-BA13AD14A20E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5020D2FC-34FC-4E93-AA99-BA13AD14A20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="11">
   <si>
     <t>Experiment</t>
   </si>
@@ -482,521 +482,587 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5132E43-9F62-4D64-994D-0B98A0467833}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="11.42578125" style="9"/>
-    <col min="7" max="7" width="13.5703125" style="9" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="9"/>
+    <col min="8" max="8" width="13.5703125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F2" s="9">
-        <v>1</v>
-      </c>
       <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9">
         <v>0.64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
       <c r="G3" s="9">
+        <v>2</v>
+      </c>
+      <c r="H3" s="9">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="9">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="9">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F4" s="9">
-        <v>3</v>
-      </c>
       <c r="G4" s="9">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9">
         <v>0.61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="9">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="9">
         <v>9.4</v>
       </c>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
       <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
         <v>0.38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="9">
         <v>9.4</v>
       </c>
-      <c r="F6" s="9">
-        <v>2</v>
-      </c>
       <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9">
         <v>0.59</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="9">
         <v>9.4</v>
       </c>
-      <c r="F7" s="9">
-        <v>3</v>
-      </c>
       <c r="G7" s="9">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9">
         <v>0.54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
       <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F9" s="9">
-        <v>2</v>
-      </c>
       <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9">
         <v>0.31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F10" s="9">
-        <v>3</v>
-      </c>
       <c r="G10" s="9">
+        <v>3</v>
+      </c>
+      <c r="H10" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="9">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9">
         <v>8.9</v>
       </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
       <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="9">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="9">
         <v>8.9</v>
       </c>
-      <c r="F12" s="9">
-        <v>2</v>
-      </c>
       <c r="G12" s="9">
+        <v>2</v>
+      </c>
+      <c r="H12" s="9">
         <v>0.43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="9">
         <v>8.9</v>
       </c>
-      <c r="F13" s="9">
-        <v>3</v>
-      </c>
       <c r="G13" s="9">
+        <v>3</v>
+      </c>
+      <c r="H13" s="9">
         <v>0.52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="9">
         <v>6.8</v>
       </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
       <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
         <v>0.39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="9">
         <v>6.8</v>
       </c>
-      <c r="F15" s="9">
-        <v>2</v>
-      </c>
       <c r="G15" s="9">
+        <v>2</v>
+      </c>
+      <c r="H15" s="9">
         <v>0.38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="9">
         <v>6.8</v>
       </c>
-      <c r="F16" s="9">
-        <v>3</v>
-      </c>
       <c r="G16" s="9">
+        <v>3</v>
+      </c>
+      <c r="H16" s="9">
         <v>0.22</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="9">
         <v>6.8</v>
       </c>
-      <c r="F17" s="9">
-        <v>1</v>
-      </c>
       <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9">
         <v>0.36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="6">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="9">
         <v>6.8</v>
       </c>
-      <c r="F18" s="9">
-        <v>2</v>
-      </c>
       <c r="G18" s="9">
+        <v>2</v>
+      </c>
+      <c r="H18" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="9">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="9">
         <v>6.8</v>
       </c>
-      <c r="F19" s="9">
-        <v>3</v>
-      </c>
       <c r="G19" s="9">
+        <v>3</v>
+      </c>
+      <c r="H19" s="9">
         <v>0.53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5">
-        <v>3</v>
-      </c>
-      <c r="C20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>3</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="10">
         <v>7.1</v>
       </c>
-      <c r="F20" s="9">
-        <v>1</v>
-      </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10">
         <v>0.42</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5">
-        <v>3</v>
-      </c>
-      <c r="C21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="10">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="10">
         <v>7.1</v>
       </c>
-      <c r="F21" s="9">
-        <v>2</v>
-      </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
+        <v>2</v>
+      </c>
+      <c r="H21" s="10">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="10">
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="10">
         <v>7.1</v>
       </c>
-      <c r="F22" s="9">
-        <v>3</v>
-      </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
+        <v>3</v>
+      </c>
+      <c r="H22" s="10">
         <v>0.42</v>
       </c>
     </row>

</xml_diff>